<commit_message>
reafactor: change Transportadora column to Importadora
</commit_message>
<xml_diff>
--- a/public/Templates/saida.xlsx
+++ b/public/Templates/saida.xlsx
@@ -19,7 +19,7 @@
     <t>Código</t>
   </si>
   <si>
-    <t>Transportadora</t>
+    <t>Importadora</t>
   </si>
   <si>
     <t>Quantidade</t>
@@ -58,7 +58,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,6 +68,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -97,31 +103,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -141,10 +147,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -165,6 +171,7 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ff68d293"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -364,12 +371,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -401,10 +408,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -643,12 +650,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -952,10 +959,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1205,7 +1212,7 @@
   <cols>
     <col min="1" max="1" width="12.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5391" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="1" customWidth="1"/>

</xml_diff>